<commit_message>
Add responsive layout for different screen widths
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -53,12 +53,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fccf45"/>
-        <bgColor rgb="00fccf45"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00fd1de9"/>
         <bgColor rgb="00fd1de9"/>
       </patternFill>
@@ -67,6 +61,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00fd4343"/>
         <bgColor rgb="00fd4343"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00fccf45"/>
+        <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
   </fills>
@@ -469,11 +469,7 @@
           <t>Name :</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>test 3</t>
-        </is>
-      </c>
+      <c r="B1" s="1" t="inlineStr"/>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Age :</t>
@@ -489,7 +485,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -497,11 +493,7 @@
           <t>Description :</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>sSda</t>
-        </is>
-      </c>
+      <c r="H1" s="1" t="inlineStr"/>
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Time of creation :</t>
@@ -509,7 +501,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Mon Mar 25 20:03:23 2024</t>
+          <t>Tue Apr  2 23:32:47 2024</t>
         </is>
       </c>
     </row>
@@ -520,7 +512,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -529,7 +521,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>99 %</t>
+          <t>11 %</t>
         </is>
       </c>
     </row>
@@ -550,7 +542,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="n"/>
       <c r="F3" s="2" t="n"/>
@@ -566,7 +558,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -586,16 +578,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -606,16 +598,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -626,7 +618,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -646,16 +638,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -666,16 +658,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D9" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -686,16 +678,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -706,16 +698,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -726,7 +718,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -746,7 +738,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -776,7 +768,7 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2" t="n"/>
       <c r="F14" s="2" t="n"/>
@@ -792,16 +784,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D15" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -812,7 +804,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -832,16 +824,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -852,16 +844,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -872,16 +864,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D19" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -899,9 +891,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -912,7 +904,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -921,7 +913,7 @@
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -932,16 +924,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D22" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -952,7 +944,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -972,7 +964,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -992,16 +984,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D25" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1012,7 +1004,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1032,7 +1024,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1059,9 +1051,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D28" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1105,9 +1097,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D30" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1118,16 +1110,16 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D31" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1130,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1158,16 +1150,16 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D33" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1178,7 +1170,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1205,9 +1197,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D35" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1210,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1238,7 +1230,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1258,7 +1250,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1288,7 +1280,7 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E39" s="2" t="n"/>
       <c r="F39" s="2" t="n"/>
@@ -1304,7 +1296,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1324,7 +1316,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1344,16 +1336,16 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D42" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1356,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1384,7 +1376,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1404,7 +1396,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1424,16 +1416,16 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D46" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1444,7 +1436,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1464,16 +1456,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D48" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1494,7 +1486,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E49" s="2" t="n"/>
       <c r="F49" s="2" t="n"/>
@@ -1510,16 +1502,16 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D50" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1530,7 +1522,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1550,16 +1542,16 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D52" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1577,9 +1569,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D53" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1590,16 +1582,16 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D54" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1610,16 +1602,16 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D55" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D55" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1630,7 +1622,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1650,16 +1642,16 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D57" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D57" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1670,16 +1662,16 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D58" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1690,16 +1682,16 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D59" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1710,16 +1702,16 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D60" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D60" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1730,7 +1722,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1750,16 +1742,16 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D62" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D62" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1770,16 +1762,16 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D63" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D63" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1800,7 +1792,7 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E64" s="2" t="n"/>
       <c r="F64" s="2" t="n"/>
@@ -1816,7 +1808,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1836,7 +1828,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1856,7 +1848,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1876,16 +1868,16 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D68" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D68" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1923,9 +1915,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D70" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D70" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1946,7 +1938,7 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E71" s="2" t="n"/>
       <c r="F71" s="2" t="n"/>
@@ -1962,16 +1954,16 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D72" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D72" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1982,7 +1974,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2002,16 +1994,16 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D74" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D74" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2022,7 +2014,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2042,16 +2034,16 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D76" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D76" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2069,9 +2061,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D77" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D77" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2082,16 +2074,16 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D78" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D78" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2102,16 +2094,16 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D79" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D79" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2114,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2142,16 +2134,16 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D81" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D81" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2172,7 +2164,7 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E82" s="2" t="n"/>
       <c r="F82" s="2" t="n"/>
@@ -2188,16 +2180,16 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D83" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D83" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2208,16 +2200,16 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D84" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D84" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2228,16 +2220,16 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D85" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D85" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2248,7 +2240,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2268,7 +2260,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2295,9 +2287,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D88" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D88" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2308,16 +2300,16 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D89" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D89" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2328,16 +2320,16 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D90" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D90" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2348,16 +2340,16 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D91" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D91" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2368,16 +2360,16 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D92" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D92" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2398,7 +2390,7 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E93" s="2" t="n"/>
       <c r="F93" s="2" t="n"/>
@@ -2414,14 +2406,14 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D94" s="4" t="inlineStr">
+      <c r="D94" s="6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2434,7 +2426,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2454,16 +2446,16 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D96" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D96" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2474,16 +2466,16 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D97" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D97" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2494,7 +2486,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2514,16 +2506,16 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D99" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D99" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2534,16 +2526,16 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D100" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D100" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2554,7 +2546,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -2574,16 +2566,16 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D102" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D102" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2621,9 +2613,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D104" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D104" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2644,7 +2636,7 @@
         </is>
       </c>
       <c r="D105" s="2" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E105" s="2" t="n"/>
       <c r="F105" s="2" t="n"/>
@@ -2660,16 +2652,16 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D106" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D106" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2680,16 +2672,16 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D107" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D107" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2700,16 +2692,16 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D108" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D108" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2720,7 +2712,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2747,9 +2739,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D110" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D110" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2760,7 +2752,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -2780,16 +2772,16 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D112" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D112" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2800,7 +2792,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -2820,16 +2812,16 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D114" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D114" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2840,16 +2832,16 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D115" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D115" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2860,16 +2852,16 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D116" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D116" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2880,16 +2872,16 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D117" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D117" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2900,7 +2892,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -2920,7 +2912,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -2970,7 +2962,7 @@
         </is>
       </c>
       <c r="D121" s="2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E121" s="2" t="n"/>
       <c r="F121" s="2" t="n"/>
@@ -2986,16 +2978,16 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D122" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D122" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3006,16 +2998,16 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D123" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D123" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3026,7 +3018,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3046,7 +3038,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -3066,16 +3058,16 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D126" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D126" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3086,16 +3078,16 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D127" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D127" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3106,7 +3098,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -3126,16 +3118,16 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D129" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D129" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3156,7 +3148,7 @@
         </is>
       </c>
       <c r="D130" s="2" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E130" s="2" t="n"/>
       <c r="F130" s="2" t="n"/>
@@ -3172,7 +3164,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -3192,16 +3184,16 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D132" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D132" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3219,9 +3211,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D133" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D133" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3252,16 +3244,16 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D135" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D135" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3272,7 +3264,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -3302,7 +3294,7 @@
         </is>
       </c>
       <c r="D137" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E137" s="2" t="n"/>
       <c r="F137" s="2" t="n"/>
@@ -3327,7 +3319,7 @@
       </c>
       <c r="D138" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3338,16 +3330,16 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D139" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D139" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3358,16 +3350,16 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D140" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D140" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3378,16 +3370,16 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D141" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D141" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3398,7 +3390,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -3418,7 +3410,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Refactor UI layout and add exception handling for screen width
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -53,20 +53,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fd1de9"/>
-        <bgColor rgb="00fd1de9"/>
+        <fgColor rgb="00fccf45"/>
+        <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00fd4343"/>
         <bgColor rgb="00fd4343"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fccf45"/>
-        <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
   </fills>
@@ -82,14 +76,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -476,7 +469,7 @@
         </is>
       </c>
       <c r="D1" s="1" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
@@ -485,7 +478,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -501,7 +494,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Tue Apr  2 23:32:47 2024</t>
+          <t>Tue Apr  2 23:55:26 2024</t>
         </is>
       </c>
     </row>
@@ -542,7 +535,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="n"/>
       <c r="F3" s="2" t="n"/>
@@ -605,9 +598,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -768,7 +761,7 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2" t="n"/>
       <c r="F14" s="2" t="n"/>
@@ -831,9 +824,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D17" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -851,9 +844,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D18" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -891,9 +884,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D20" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -911,9 +904,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D21" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1067,7 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2" t="n"/>
       <c r="F29" s="2" t="n"/>
@@ -1097,9 +1090,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D30" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1157,9 +1150,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D33" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1479,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" s="2" t="n"/>
       <c r="F49" s="2" t="n"/>
@@ -1509,7 +1502,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D50" s="6" t="inlineStr">
+      <c r="D50" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -1569,9 +1562,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D53" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1589,9 +1582,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D54" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1609,9 +1602,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D55" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D55" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1931,7 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E71" s="2" t="n"/>
       <c r="F71" s="2" t="n"/>
@@ -2061,9 +2054,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D77" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D77" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2164,7 +2157,7 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E82" s="2" t="n"/>
       <c r="F82" s="2" t="n"/>
@@ -2187,9 +2180,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D83" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D83" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2207,9 +2200,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D84" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D84" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2383,7 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E93" s="2" t="n"/>
       <c r="F93" s="2" t="n"/>
@@ -2413,9 +2406,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D94" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D94" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2453,9 +2446,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D96" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D96" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2473,9 +2466,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D97" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D97" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2636,7 +2629,7 @@
         </is>
       </c>
       <c r="D105" s="2" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E105" s="2" t="n"/>
       <c r="F105" s="2" t="n"/>
@@ -2659,9 +2652,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D106" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D106" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2679,9 +2672,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D107" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D107" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2699,7 +2692,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D108" s="6" t="inlineStr">
+      <c r="D108" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2739,9 +2732,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D110" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D110" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2759,9 +2752,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D111" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D111" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2962,7 +2955,7 @@
         </is>
       </c>
       <c r="D121" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E121" s="2" t="n"/>
       <c r="F121" s="2" t="n"/>
@@ -3005,9 +2998,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D123" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D123" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3294,7 +3287,7 @@
         </is>
       </c>
       <c r="D137" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E137" s="2" t="n"/>
       <c r="F137" s="2" t="n"/>
@@ -3317,7 +3310,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D138" s="6" t="inlineStr">
+      <c r="D138" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -3377,9 +3370,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D141" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D141" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove unused Streamlit configuration file
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -53,14 +53,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00fd4343"/>
+        <bgColor rgb="00fd4343"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00fccf45"/>
         <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fd4343"/>
-        <bgColor rgb="00fd4343"/>
+        <fgColor rgb="00fd1de9"/>
+        <bgColor rgb="00fd1de9"/>
       </patternFill>
     </fill>
   </fills>
@@ -76,13 +82,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -469,7 +476,7 @@
         </is>
       </c>
       <c r="D1" s="1" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
@@ -478,7 +485,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -494,7 +501,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Tue Apr  2 23:55:26 2024</t>
+          <t>Sun Apr 14 23:04:00 2024</t>
         </is>
       </c>
     </row>
@@ -505,7 +512,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -514,7 +521,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11 %</t>
+          <t>91 %</t>
         </is>
       </c>
     </row>
@@ -535,7 +542,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="n"/>
       <c r="F3" s="2" t="n"/>
@@ -551,7 +558,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -571,7 +578,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -591,16 +598,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -611,7 +618,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -631,7 +638,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -651,7 +658,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -671,7 +678,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -691,7 +698,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -711,7 +718,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -731,16 +738,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -761,7 +768,7 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2" t="n"/>
       <c r="F14" s="2" t="n"/>
@@ -777,7 +784,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -797,7 +804,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -817,7 +824,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -837,16 +844,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -857,7 +864,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -897,7 +904,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -917,7 +924,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -937,7 +944,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -957,7 +964,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -977,7 +984,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -997,16 +1004,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D26" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1024,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1044,9 +1051,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D28" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1103,7 +1110,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1123,7 +1130,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1143,7 +1150,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1163,7 +1170,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1203,7 +1210,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1223,7 +1230,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1243,7 +1250,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1273,7 +1280,7 @@
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" s="2" t="n"/>
       <c r="F39" s="2" t="n"/>
@@ -1289,7 +1296,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1309,7 +1316,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1329,7 +1336,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1349,16 +1356,16 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D43" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D43" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1376,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1389,7 +1396,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1409,7 +1416,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1429,7 +1436,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1449,7 +1456,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1479,7 +1486,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E49" s="2" t="n"/>
       <c r="F49" s="2" t="n"/>
@@ -1495,16 +1502,16 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D50" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1515,7 +1522,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1535,7 +1542,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1575,16 +1582,16 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D54" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1602,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1615,7 +1622,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1635,7 +1642,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1655,16 +1662,16 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D58" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D58" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1682,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1695,7 +1702,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1715,7 +1722,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1735,16 +1742,16 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D62" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D62" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1755,7 +1762,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1801,7 +1808,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1821,7 +1828,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1841,7 +1848,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1861,7 +1868,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1931,7 +1938,7 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E71" s="2" t="n"/>
       <c r="F71" s="2" t="n"/>
@@ -1947,7 +1954,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -1967,7 +1974,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -1987,7 +1994,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2007,16 +2014,16 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D75" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2034,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2067,7 +2074,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2087,7 +2094,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2107,16 +2114,16 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D80" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D80" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2134,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2157,7 +2164,7 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E82" s="2" t="n"/>
       <c r="F82" s="2" t="n"/>
@@ -2173,16 +2180,16 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D83" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D83" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2200,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2202,7 +2209,7 @@
       </c>
       <c r="D84" s="4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2220,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2233,7 +2240,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2253,7 +2260,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2293,7 +2300,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2313,7 +2320,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2333,7 +2340,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2353,7 +2360,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2383,7 +2390,7 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E93" s="2" t="n"/>
       <c r="F93" s="2" t="n"/>
@@ -2399,16 +2406,16 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D94" s="5" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D94" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2426,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2439,7 +2446,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2459,16 +2466,16 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D97" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D97" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2479,7 +2486,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2499,7 +2506,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -2519,7 +2526,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -2539,7 +2546,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -2559,7 +2566,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -2586,9 +2593,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D103" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D103" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2606,9 +2613,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D104" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D104" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2636,7 @@
         </is>
       </c>
       <c r="D105" s="2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E105" s="2" t="n"/>
       <c r="F105" s="2" t="n"/>
@@ -2645,7 +2652,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -2665,7 +2672,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -2685,16 +2692,16 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D108" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D108" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2705,7 +2712,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2745,16 +2752,16 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D111" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D111" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2765,7 +2772,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -2785,7 +2792,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -2805,7 +2812,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -2825,7 +2832,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -2845,16 +2852,16 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D116" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D116" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2865,16 +2872,16 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D117" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D117" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2885,16 +2892,16 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D118" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D118" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2905,7 +2912,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -2932,9 +2939,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D120" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D120" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2955,7 +2962,7 @@
         </is>
       </c>
       <c r="D121" s="2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E121" s="2" t="n"/>
       <c r="F121" s="2" t="n"/>
@@ -2971,7 +2978,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -2991,7 +2998,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3011,7 +3018,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3031,16 +3038,16 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D125" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D125" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3051,7 +3058,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -3071,16 +3078,16 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D127" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D127" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3098,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -3111,7 +3118,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -3157,7 +3164,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -3177,7 +3184,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -3237,7 +3244,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -3257,7 +3264,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -3287,7 +3294,7 @@
         </is>
       </c>
       <c r="D137" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E137" s="2" t="n"/>
       <c r="F137" s="2" t="n"/>
@@ -3310,9 +3317,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D138" s="4" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D138" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3323,7 +3330,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -3343,7 +3350,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -3363,7 +3370,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -3383,7 +3390,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -3403,7 +3410,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Refactor Survey class to improve code readability and maintainability
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -59,14 +59,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fccf45"/>
-        <bgColor rgb="00fccf45"/>
+        <fgColor rgb="00fd1de9"/>
+        <bgColor rgb="00fd1de9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fd1de9"/>
-        <bgColor rgb="00fd1de9"/>
+        <fgColor rgb="00fccf45"/>
+        <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
   </fills>
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J143"/>
+  <dimension ref="A1:J178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,55 +501,55 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Sun Apr 14 23:04:00 2024</t>
+          <t>Mon Apr 15 20:38:36 2024</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>ADHD Index score :</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Probability of ADHD :</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>91 %</t>
-        </is>
-      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>41 %</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="n"/>
-      <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="n"/>
-      <c r="H3" s="2" t="n"/>
-      <c r="I3" s="2" t="n"/>
-      <c r="J3" s="2" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>101</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -698,16 +698,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -732,50 +732,56 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>88</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Oppositional defiant disorder score :</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Oppositional defiant disorder :</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="n"/>
+      <c r="I13" s="2" t="n"/>
+      <c r="J13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>HY</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2" t="n"/>
-      <c r="F14" s="2" t="n"/>
-      <c r="G14" s="2" t="n"/>
-      <c r="H14" s="2" t="n"/>
-      <c r="I14" s="2" t="n"/>
-      <c r="J14" s="2" t="n"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>21</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -784,7 +790,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -793,8 +799,16 @@
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -804,17 +818,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -824,7 +846,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -833,8 +855,16 @@
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -844,17 +874,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D18" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -864,17 +902,25 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -884,7 +930,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -893,8 +939,16 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -904,38 +958,50 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D21" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>19</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Behavior disorder score :</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>Behavior disorder :</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
+      <c r="H22" s="2" t="n"/>
+      <c r="I22" s="2" t="n"/>
+      <c r="J22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -944,7 +1010,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -953,8 +1019,16 @@
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -964,17 +1038,25 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -984,17 +1066,25 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D25" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1004,7 +1094,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1013,8 +1103,16 @@
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1024,17 +1122,25 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D27" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1044,44 +1150,54 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D28" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>LP</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D29" s="2" t="n">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>78</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F29" t="b">
         <v>0</v>
       </c>
-      <c r="E29" s="2" t="n"/>
-      <c r="F29" s="2" t="n"/>
-      <c r="G29" s="2" t="n"/>
-      <c r="H29" s="2" t="n"/>
-      <c r="I29" s="2" t="n"/>
-      <c r="J29" s="2" t="n"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1090,17 +1206,25 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D30" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1110,17 +1234,25 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D31" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1130,17 +1262,25 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D32" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1150,17 +1290,25 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D33" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D33" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1170,17 +1318,25 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D34" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D34" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1190,17 +1346,25 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D35" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D35" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1210,17 +1374,25 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D36" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D36" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1230,64 +1402,72 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D37" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D37" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>60</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D38" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2" t="n"/>
+      <c r="F38" s="2" t="n"/>
+      <c r="G38" s="2" t="n"/>
+      <c r="H38" s="2" t="n"/>
+      <c r="I38" s="2" t="n"/>
+      <c r="J38" s="2" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B39" s="2" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="C39" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E39" s="2" t="n"/>
-      <c r="F39" s="2" t="n"/>
-      <c r="G39" s="2" t="n"/>
-      <c r="H39" s="2" t="n"/>
-      <c r="I39" s="2" t="n"/>
-      <c r="J39" s="2" t="n"/>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>49</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1296,7 +1476,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1316,16 +1496,16 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D41" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D41" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1516,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1356,16 +1536,16 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D43" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1556,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1396,7 +1576,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1416,7 +1596,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1436,16 +1616,16 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D47" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1456,16 +1636,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D48" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1657,7 @@
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>AG</t>
+          <t>HY</t>
         </is>
       </c>
       <c r="C49" s="2" t="inlineStr">
@@ -1486,7 +1666,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E49" s="2" t="n"/>
       <c r="F49" s="2" t="n"/>
@@ -1502,7 +1682,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1522,7 +1702,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1542,16 +1722,16 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D52" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D52" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1562,7 +1742,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1582,7 +1762,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1602,7 +1782,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1622,7 +1802,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1642,7 +1822,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1662,16 +1842,16 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D58" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1862,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1702,7 +1882,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1722,7 +1902,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1742,16 +1922,16 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D62" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D62" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1762,7 +1942,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1783,7 +1963,7 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>LP</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
@@ -1792,7 +1972,7 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E64" s="2" t="n"/>
       <c r="F64" s="2" t="n"/>
@@ -1808,7 +1988,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1828,7 +2008,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1848,7 +2028,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1868,7 +2048,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1888,16 +2068,16 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D69" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D69" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1908,7 +2088,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -1922,30 +2102,24 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B71" s="2" t="inlineStr">
-        <is>
-          <t>GI</t>
-        </is>
-      </c>
-      <c r="C71" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D71" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E71" s="2" t="n"/>
-      <c r="F71" s="2" t="n"/>
-      <c r="G71" s="2" t="n"/>
-      <c r="H71" s="2" t="n"/>
-      <c r="I71" s="2" t="n"/>
-      <c r="J71" s="2" t="n"/>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>87</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D71" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1954,7 +2128,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -1974,7 +2148,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -1988,24 +2162,30 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>81</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D74" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" s="2" t="n"/>
+      <c r="F74" s="2" t="n"/>
+      <c r="G74" s="2" t="n"/>
+      <c r="H74" s="2" t="n"/>
+      <c r="I74" s="2" t="n"/>
+      <c r="J74" s="2" t="n"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2014,16 +2194,16 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D75" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D75" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2034,7 +2214,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2054,7 +2234,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2074,7 +2254,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2094,7 +2274,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2114,16 +2294,16 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D80" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D80" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2134,7 +2314,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2148,30 +2328,24 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B82" s="2" t="inlineStr">
-        <is>
-          <t>AN</t>
-        </is>
-      </c>
-      <c r="C82" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D82" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E82" s="2" t="n"/>
-      <c r="F82" s="2" t="n"/>
-      <c r="G82" s="2" t="n"/>
-      <c r="H82" s="2" t="n"/>
-      <c r="I82" s="2" t="n"/>
-      <c r="J82" s="2" t="n"/>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>72</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D82" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2180,7 +2354,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2194,24 +2368,30 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
-        <v>101</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D84" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>AG</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E84" s="2" t="n"/>
+      <c r="F84" s="2" t="n"/>
+      <c r="G84" s="2" t="n"/>
+      <c r="H84" s="2" t="n"/>
+      <c r="I84" s="2" t="n"/>
+      <c r="J84" s="2" t="n"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2220,16 +2400,16 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D85" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D85" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2240,7 +2420,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2260,7 +2440,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2280,7 +2460,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2300,7 +2480,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2320,16 +2500,16 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D90" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D90" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2340,16 +2520,16 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D91" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D91" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2360,7 +2540,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2374,30 +2554,24 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B93" s="2" t="inlineStr">
-        <is>
-          <t>AH</t>
-        </is>
-      </c>
-      <c r="C93" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E93" s="2" t="n"/>
-      <c r="F93" s="2" t="n"/>
-      <c r="G93" s="2" t="n"/>
-      <c r="H93" s="2" t="n"/>
-      <c r="I93" s="2" t="n"/>
-      <c r="J93" s="2" t="n"/>
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>102</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2406,7 +2580,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2426,7 +2600,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2446,7 +2620,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2466,16 +2640,16 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D97" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D97" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2486,7 +2660,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2500,24 +2674,30 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B99" t="n">
-        <v>98</v>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D99" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B99" s="2" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E99" s="2" t="n"/>
+      <c r="F99" s="2" t="n"/>
+      <c r="G99" s="2" t="n"/>
+      <c r="H99" s="2" t="n"/>
+      <c r="I99" s="2" t="n"/>
+      <c r="J99" s="2" t="n"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2526,7 +2706,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -2546,7 +2726,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -2566,7 +2746,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -2586,14 +2766,14 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D103" s="5" t="inlineStr">
+      <c r="D103" s="6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2606,64 +2786,64 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D104" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D104" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="inlineStr">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>92</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D105" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
         <is>
           <t>Category :</t>
         </is>
       </c>
-      <c r="B105" s="2" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="C105" s="2" t="inlineStr">
+      <c r="B106" s="2" t="inlineStr">
+        <is>
+          <t>GI</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
         <is>
           <t>Overall score :</t>
         </is>
       </c>
-      <c r="D105" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E105" s="2" t="n"/>
-      <c r="F105" s="2" t="n"/>
-      <c r="G105" s="2" t="n"/>
-      <c r="H105" s="2" t="n"/>
-      <c r="I105" s="2" t="n"/>
-      <c r="J105" s="2" t="n"/>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B106" t="n">
-        <v>41</v>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D106" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="D106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" s="2" t="n"/>
+      <c r="F106" s="2" t="n"/>
+      <c r="G106" s="2" t="n"/>
+      <c r="H106" s="2" t="n"/>
+      <c r="I106" s="2" t="n"/>
+      <c r="J106" s="2" t="n"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2672,7 +2852,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -2692,7 +2872,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -2712,7 +2892,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2732,7 +2912,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -2752,7 +2932,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -2772,7 +2952,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -2792,7 +2972,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -2812,7 +2992,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -2832,7 +3012,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -2852,38 +3032,44 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D116" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D116" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B117" t="n">
-        <v>16</v>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D117" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="A117" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B117" s="2" t="inlineStr">
+        <is>
+          <t>AN</t>
+        </is>
+      </c>
+      <c r="C117" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="2" t="n"/>
+      <c r="F117" s="2" t="n"/>
+      <c r="G117" s="2" t="n"/>
+      <c r="H117" s="2" t="n"/>
+      <c r="I117" s="2" t="n"/>
+      <c r="J117" s="2" t="n"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2892,16 +3078,16 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D118" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D118" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2912,7 +3098,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -2932,44 +3118,38 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D120" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D120" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B121" s="2" t="inlineStr">
-        <is>
-          <t>OD</t>
-        </is>
-      </c>
-      <c r="C121" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D121" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E121" s="2" t="n"/>
-      <c r="F121" s="2" t="n"/>
-      <c r="G121" s="2" t="n"/>
-      <c r="H121" s="2" t="n"/>
-      <c r="I121" s="2" t="n"/>
-      <c r="J121" s="2" t="n"/>
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>35</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D121" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2978,7 +3158,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -2998,7 +3178,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3018,7 +3198,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3038,16 +3218,16 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D125" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D125" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3058,7 +3238,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -3078,38 +3258,44 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D127" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D127" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B128" t="n">
-        <v>59</v>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D128" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A128" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B128" s="2" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="C128" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D128" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E128" s="2" t="n"/>
+      <c r="F128" s="2" t="n"/>
+      <c r="G128" s="2" t="n"/>
+      <c r="H128" s="2" t="n"/>
+      <c r="I128" s="2" t="n"/>
+      <c r="J128" s="2" t="n"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3118,7 +3304,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -3132,30 +3318,24 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B130" s="2" t="inlineStr">
-        <is>
-          <t>PI</t>
-        </is>
-      </c>
-      <c r="C130" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E130" s="2" t="n"/>
-      <c r="F130" s="2" t="n"/>
-      <c r="G130" s="2" t="n"/>
-      <c r="H130" s="2" t="n"/>
-      <c r="I130" s="2" t="n"/>
-      <c r="J130" s="2" t="n"/>
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>61</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D130" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3164,16 +3344,16 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D131" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D131" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3364,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -3204,7 +3384,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -3224,7 +3404,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -3244,7 +3424,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -3264,7 +3444,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -3278,30 +3458,24 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B137" s="2" t="inlineStr">
-        <is>
-          <t>NI</t>
-        </is>
-      </c>
-      <c r="C137" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D137" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E137" s="2" t="n"/>
-      <c r="F137" s="2" t="n"/>
-      <c r="G137" s="2" t="n"/>
-      <c r="H137" s="2" t="n"/>
-      <c r="I137" s="2" t="n"/>
-      <c r="J137" s="2" t="n"/>
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>71</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D137" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3310,7 +3484,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -3330,7 +3504,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -3344,24 +3518,30 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B140" t="n">
-        <v>26</v>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D140" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A140" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B140" s="2" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="C140" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D140" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E140" s="2" t="n"/>
+      <c r="F140" s="2" t="n"/>
+      <c r="G140" s="2" t="n"/>
+      <c r="H140" s="2" t="n"/>
+      <c r="I140" s="2" t="n"/>
+      <c r="J140" s="2" t="n"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3370,16 +3550,16 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D141" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D141" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3390,7 +3570,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -3410,14 +3590,732 @@
         </is>
       </c>
       <c r="B143" t="n">
+        <v>89</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D143" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>6</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D144" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>30</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D145" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>58</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D146" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>78</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D147" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>11</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D148" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>27</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D149" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>39</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D150" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>91</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D151" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>16</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D152" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>56</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D153" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>76</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D154" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>96</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D155" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B156" s="2" t="inlineStr">
+        <is>
+          <t>OD</t>
+        </is>
+      </c>
+      <c r="C156" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D156" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E156" s="2" t="n"/>
+      <c r="F156" s="2" t="n"/>
+      <c r="G156" s="2" t="n"/>
+      <c r="H156" s="2" t="n"/>
+      <c r="I156" s="2" t="n"/>
+      <c r="J156" s="2" t="n"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>21</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D157" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>57</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D158" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>73</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D159" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>14</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D160" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>94</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D161" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>102</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D162" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>59</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D163" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>48</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D164" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B165" s="2" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="C165" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D165" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" s="2" t="n"/>
+      <c r="F165" s="2" t="n"/>
+      <c r="G165" s="2" t="n"/>
+      <c r="H165" s="2" t="n"/>
+      <c r="I165" s="2" t="n"/>
+      <c r="J165" s="2" t="n"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>33</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D166" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>105</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D167" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>38</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D168" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>74</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D169" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>31</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D170" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>80</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D171" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B172" s="2" t="inlineStr">
+        <is>
+          <t>NI</t>
+        </is>
+      </c>
+      <c r="C172" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D172" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E172" s="2" t="n"/>
+      <c r="F172" s="2" t="n"/>
+      <c r="G172" s="2" t="n"/>
+      <c r="H172" s="2" t="n"/>
+      <c r="I172" s="2" t="n"/>
+      <c r="J172" s="2" t="n"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>1</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D173" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>18</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D174" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>26</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D175" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>42</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D176" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>8</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D177" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
         <v>32</v>
       </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D143" s="3" t="inlineStr">
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D178" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Fix typo in Answer class initialization
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -53,6 +53,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00fccf45"/>
+        <bgColor rgb="00fccf45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00fd4343"/>
         <bgColor rgb="00fd4343"/>
       </patternFill>
@@ -61,12 +67,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00fd1de9"/>
         <bgColor rgb="00fd1de9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fccf45"/>
-        <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
   </fills>
@@ -501,7 +501,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Mon Apr 15 20:38:36 2024</t>
+          <t>Mon Apr 15 21:03:27 2024</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>41 %</t>
+          <t>97 %</t>
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
@@ -605,9 +605,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -625,9 +625,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -645,9 +645,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -665,9 +665,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D11" s="4" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="n"/>
       <c r="F13" s="2" t="n"/>
@@ -769,7 +769,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D14" s="5" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -825,7 +825,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D16" s="5" t="inlineStr">
+      <c r="D16" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -881,9 +881,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D18" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D18" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -909,9 +909,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D19" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -965,9 +965,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D21" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D21" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="n"/>
       <c r="F22" s="2" t="n"/>
@@ -1045,9 +1045,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D24" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1056,7 +1056,7 @@
         </is>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1073,7 +1073,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D25" s="5" t="inlineStr">
+      <c r="D25" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1101,7 +1101,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D26" s="5" t="inlineStr">
+      <c r="D26" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1129,9 +1129,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D27" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="F27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1185,9 +1185,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D29" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="F29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1213,7 +1213,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D30" s="5" t="inlineStr">
+      <c r="D30" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1241,9 +1241,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D31" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="F31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1269,9 +1269,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D32" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1280,7 +1280,7 @@
         </is>
       </c>
       <c r="F32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1297,9 +1297,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D33" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1325,7 +1325,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D34" s="5" t="inlineStr">
+      <c r="D34" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1353,9 +1353,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D35" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1364,7 +1364,7 @@
         </is>
       </c>
       <c r="F35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1381,9 +1381,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D36" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="F36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1409,7 +1409,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D37" s="5" t="inlineStr">
+      <c r="D37" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1440,7 +1440,7 @@
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E38" s="2" t="n"/>
       <c r="F38" s="2" t="n"/>
@@ -1463,9 +1463,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D39" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D39" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1483,9 +1483,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D40" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D40" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1503,7 +1503,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D41" s="6" t="inlineStr">
+      <c r="D41" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -1523,9 +1523,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D42" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1543,9 +1543,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D43" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D43" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1563,9 +1563,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D44" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D44" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1603,9 +1603,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D47" s="6" t="inlineStr">
+      <c r="D47" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -1643,7 +1643,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D48" s="4" t="inlineStr">
+      <c r="D48" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -1666,7 +1666,7 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E49" s="2" t="n"/>
       <c r="F49" s="2" t="n"/>
@@ -1709,9 +1709,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D51" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D51" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1729,7 +1729,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D52" s="4" t="inlineStr">
+      <c r="D52" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -1769,9 +1769,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D54" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1869,9 +1869,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D59" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D59" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1909,9 +1909,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D61" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D61" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1929,9 +1929,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D62" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D62" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E64" s="2" t="n"/>
       <c r="F64" s="2" t="n"/>
@@ -2075,7 +2075,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D69" s="4" t="inlineStr">
+      <c r="D69" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2095,9 +2095,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D70" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D70" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D71" s="4" t="inlineStr">
+      <c r="D71" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2135,9 +2135,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D72" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D72" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2178,7 +2178,7 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E74" s="2" t="n"/>
       <c r="F74" s="2" t="n"/>
@@ -2261,9 +2261,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D78" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D78" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2281,9 +2281,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D79" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D79" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2301,9 +2301,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D80" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D80" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2321,9 +2321,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D81" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D81" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D82" s="4" t="inlineStr">
+      <c r="D82" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2384,7 +2384,7 @@
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E84" s="2" t="n"/>
       <c r="F84" s="2" t="n"/>
@@ -2407,7 +2407,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D85" s="6" t="inlineStr">
+      <c r="D85" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2427,9 +2427,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D86" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D86" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2467,9 +2467,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D88" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D88" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2487,9 +2487,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D89" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D89" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D90" s="4" t="inlineStr">
+      <c r="D90" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2527,7 +2527,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D91" s="6" t="inlineStr">
+      <c r="D91" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2547,9 +2547,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D92" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D92" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2567,9 +2567,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D93" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D93" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2587,9 +2587,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D94" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D94" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2607,9 +2607,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D95" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D95" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2627,9 +2627,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D96" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D96" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2667,9 +2667,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D98" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D98" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2690,7 +2690,7 @@
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E99" s="2" t="n"/>
       <c r="F99" s="2" t="n"/>
@@ -2753,9 +2753,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D102" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D102" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D103" s="6" t="inlineStr">
+      <c r="D103" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2793,9 +2793,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D104" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D104" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2836,7 +2836,7 @@
         </is>
       </c>
       <c r="D106" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E106" s="2" t="n"/>
       <c r="F106" s="2" t="n"/>
@@ -2859,9 +2859,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D107" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D107" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2899,9 +2899,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D109" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D109" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2919,9 +2919,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D110" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D110" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2959,9 +2959,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D112" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D112" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2999,9 +2999,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D114" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D114" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3019,9 +3019,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D115" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D115" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3062,7 +3062,7 @@
         </is>
       </c>
       <c r="D117" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E117" s="2" t="n"/>
       <c r="F117" s="2" t="n"/>
@@ -3145,9 +3145,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D121" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D121" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3165,9 +3165,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D122" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D122" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3185,9 +3185,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D123" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D123" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3205,9 +3205,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D124" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D124" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3225,9 +3225,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D125" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D125" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3245,9 +3245,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D126" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D126" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3288,7 +3288,7 @@
         </is>
       </c>
       <c r="D128" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E128" s="2" t="n"/>
       <c r="F128" s="2" t="n"/>
@@ -3331,9 +3331,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D130" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D130" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3351,7 +3351,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D131" s="4" t="inlineStr">
+      <c r="D131" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -3491,9 +3491,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D138" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D138" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3534,7 +3534,7 @@
         </is>
       </c>
       <c r="D140" s="2" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E140" s="2" t="n"/>
       <c r="F140" s="2" t="n"/>
@@ -3557,7 +3557,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D141" s="6" t="inlineStr">
+      <c r="D141" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -3577,9 +3577,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D142" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D142" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3637,9 +3637,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D145" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D145" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3657,7 +3657,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D146" s="4" t="inlineStr">
+      <c r="D146" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -3677,9 +3677,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D147" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D147" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3717,9 +3717,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D149" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D149" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3737,9 +3737,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D150" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D150" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3757,9 +3757,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D151" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D151" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3797,9 +3797,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D153" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D153" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3817,9 +3817,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D154" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D154" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3860,7 +3860,7 @@
         </is>
       </c>
       <c r="D156" s="2" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E156" s="2" t="n"/>
       <c r="F156" s="2" t="n"/>
@@ -3903,7 +3903,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D158" s="6" t="inlineStr">
+      <c r="D158" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -3943,7 +3943,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D160" s="6" t="inlineStr">
+      <c r="D160" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -3963,9 +3963,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D161" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D161" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3983,9 +3983,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D162" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D162" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4003,7 +4003,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D163" s="6" t="inlineStr">
+      <c r="D163" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -4023,9 +4023,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D164" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D164" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4046,7 @@
         </is>
       </c>
       <c r="D165" s="2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E165" s="2" t="n"/>
       <c r="F165" s="2" t="n"/>
@@ -4089,9 +4089,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D167" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D167" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4109,9 +4109,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D168" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D168" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4149,9 +4149,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D170" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D170" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4169,9 +4169,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D171" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D171" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4275,7 +4275,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D176" s="4" t="inlineStr">
+      <c r="D176" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>

</xml_diff>

<commit_message>
Update cSpell dictionary with new words and add evaluation for ADHD with inattention and hyperactivity
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -57,12 +57,6 @@
         <bgColor rgb="00fd1de9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fccf45"/>
-        <bgColor rgb="00fccf45"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -76,13 +70,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -494,7 +487,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Mon Apr 15 21:36:56 2024</t>
+          <t>Wed Apr 17 14:05:13 2024</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2722,7 @@
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E99" s="2" t="n"/>
       <c r="F99" s="2" t="n"/>
@@ -2772,9 +2765,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D101" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor Survey class to add evaluation for ADHD with inattention and hyperactivity in app.py
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -53,6 +53,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00fd4343"/>
+        <bgColor rgb="00fd4343"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00fccf45"/>
+        <bgColor rgb="00fccf45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00fd1de9"/>
         <bgColor rgb="00fd1de9"/>
       </patternFill>
@@ -70,12 +82,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -441,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J178"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,7 +501,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Wed Apr 17 14:05:13 2024</t>
+          <t>Thu Apr 18 12:52:19 2024</t>
         </is>
       </c>
     </row>
@@ -498,7 +512,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -507,7 +521,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>11 %</t>
+          <t>99 %</t>
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
@@ -551,9 +565,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -591,9 +605,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -611,9 +625,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -631,9 +645,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -651,9 +665,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -691,9 +705,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -711,24 +725,24 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Oppositional defiant disorder score :</t>
+          <t>ADHD Hyperactivity score :</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Oppositional defiant disorder :</t>
+          <t>ADHD Hyperactivity :</t>
         </is>
       </c>
       <c r="D13" s="2" t="b">
@@ -748,14 +762,14 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D14" s="4" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -778,14 +792,14 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D15" s="4" t="inlineStr">
+      <c r="D15" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -808,14 +822,14 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D16" s="4" t="inlineStr">
+      <c r="D16" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -838,14 +852,14 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D17" s="4" t="inlineStr">
+      <c r="D17" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -868,16 +882,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D18" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D18" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -898,16 +912,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D19" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -917,7 +931,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -928,14 +942,14 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D20" s="4" t="inlineStr">
+      <c r="D20" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -958,16 +972,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D21" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -977,33 +991,39 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Behavior disorder score :</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Behavior disorder :</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="n"/>
-      <c r="F22" s="2" t="n"/>
-      <c r="G22" s="2" t="n"/>
-      <c r="H22" s="2" t="n"/>
-      <c r="I22" s="2" t="n"/>
-      <c r="J22" s="2" t="n"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>71</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1012,16 +1032,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D23" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D23" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1042,16 +1062,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D24" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D24" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1066,34 +1086,28 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>89</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D25" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Evaluated :</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>ADHD Inattention score :</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>ADHD Inattention :</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="n"/>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
+      <c r="H25" s="2" t="n"/>
+      <c r="I25" s="2" t="n"/>
+      <c r="J25" s="2" t="n"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1102,16 +1116,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D26" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1121,7 +1135,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1132,14 +1146,14 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D27" s="4" t="inlineStr">
+      <c r="D27" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1162,14 +1176,14 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D28" s="4" t="inlineStr">
+      <c r="D28" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1192,16 +1206,16 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D29" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1211,7 +1225,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1222,16 +1236,16 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D30" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1241,7 +1255,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1252,14 +1266,14 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D31" s="4" t="inlineStr">
+      <c r="D31" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1282,14 +1296,14 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D32" s="4" t="inlineStr">
+      <c r="D32" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1312,14 +1326,14 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D33" s="4" t="inlineStr">
+      <c r="D33" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1342,16 +1356,16 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D34" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D34" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1372,14 +1386,14 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D35" s="4" t="inlineStr">
+      <c r="D35" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1396,34 +1410,28 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>76</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D36" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Evaluated :</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Oppositional defiant disorder score :</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>Oppositional defiant disorder :</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n"/>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="n"/>
+      <c r="H36" s="2" t="n"/>
+      <c r="I36" s="2" t="n"/>
+      <c r="J36" s="2" t="n"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1432,14 +1440,14 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D37" s="4" t="inlineStr">
+      <c r="D37" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1456,30 +1464,34 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B38" s="2" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="C38" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="n"/>
-      <c r="F38" s="2" t="n"/>
-      <c r="G38" s="2" t="n"/>
-      <c r="H38" s="2" t="n"/>
-      <c r="I38" s="2" t="n"/>
-      <c r="J38" s="2" t="n"/>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>57</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D38" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1488,16 +1500,26 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D39" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D39" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1508,16 +1530,26 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D40" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D40" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1528,16 +1560,26 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D41" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D41" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1548,7 +1590,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1557,7 +1599,17 @@
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1620,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1577,7 +1629,17 @@
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1650,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1597,29 +1659,43 @@
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>12</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>Behavior disorder score :</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>Behavior disorder :</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="n"/>
+      <c r="F45" s="2" t="n"/>
+      <c r="G45" s="2" t="n"/>
+      <c r="H45" s="2" t="n"/>
+      <c r="I45" s="2" t="n"/>
+      <c r="J45" s="2" t="n"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1628,16 +1704,26 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D46" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1648,16 +1734,26 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D47" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1668,44 +1764,58 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D48" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B49" s="2" t="inlineStr">
-        <is>
-          <t>HY</t>
-        </is>
-      </c>
-      <c r="C49" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="2" t="n"/>
-      <c r="F49" s="2" t="n"/>
-      <c r="G49" s="2" t="n"/>
-      <c r="H49" s="2" t="n"/>
-      <c r="I49" s="2" t="n"/>
-      <c r="J49" s="2" t="n"/>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>6</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1714,16 +1824,26 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D50" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1734,16 +1854,26 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D51" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1754,7 +1884,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1763,7 +1893,17 @@
       </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1774,16 +1914,26 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1794,16 +1944,26 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D54" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D54" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1814,16 +1974,26 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D55" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1834,16 +2004,26 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D56" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D56" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1854,16 +2034,26 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1874,7 +2064,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1883,7 +2073,17 @@
       </c>
       <c r="D58" s="3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1894,16 +2094,26 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D59" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1914,38 +2124,54 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D60" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D60" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>false</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>99</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E61" s="2" t="n"/>
+      <c r="F61" s="2" t="n"/>
+      <c r="G61" s="2" t="n"/>
+      <c r="H61" s="2" t="n"/>
+      <c r="I61" s="2" t="n"/>
+      <c r="J61" s="2" t="n"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1954,7 +2180,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1974,44 +2200,38 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D63" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D63" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B64" s="2" t="inlineStr">
-        <is>
-          <t>LP</t>
-        </is>
-      </c>
-      <c r="C64" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E64" s="2" t="n"/>
-      <c r="F64" s="2" t="n"/>
-      <c r="G64" s="2" t="n"/>
-      <c r="H64" s="2" t="n"/>
-      <c r="I64" s="2" t="n"/>
-      <c r="J64" s="2" t="n"/>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>23</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2020,16 +2240,16 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D65" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D65" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2040,16 +2260,16 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D66" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D66" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2060,7 +2280,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2080,7 +2300,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2100,7 +2320,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2120,7 +2340,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2140,38 +2360,44 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D71" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>36</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D72" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>HY</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E72" s="2" t="n"/>
+      <c r="F72" s="2" t="n"/>
+      <c r="G72" s="2" t="n"/>
+      <c r="H72" s="2" t="n"/>
+      <c r="I72" s="2" t="n"/>
+      <c r="J72" s="2" t="n"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2180,7 +2406,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2194,30 +2420,24 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B74" s="2" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="C74" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E74" s="2" t="n"/>
-      <c r="F74" s="2" t="n"/>
-      <c r="G74" s="2" t="n"/>
-      <c r="H74" s="2" t="n"/>
-      <c r="I74" s="2" t="n"/>
-      <c r="J74" s="2" t="n"/>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>61</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2226,7 +2446,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2246,7 +2466,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2266,16 +2486,16 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D77" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D77" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2286,16 +2506,16 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D78" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D78" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2306,16 +2526,16 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D79" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D79" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2546,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2346,16 +2566,16 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D81" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D81" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2366,16 +2586,16 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D82" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D82" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2386,44 +2606,38 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D83" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D83" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B84" s="2" t="inlineStr">
-        <is>
-          <t>AG</t>
-        </is>
-      </c>
-      <c r="C84" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="n"/>
-      <c r="F84" s="2" t="n"/>
-      <c r="G84" s="2" t="n"/>
-      <c r="H84" s="2" t="n"/>
-      <c r="I84" s="2" t="n"/>
-      <c r="J84" s="2" t="n"/>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>99</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D84" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2432,16 +2646,16 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D85" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D85" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2452,38 +2666,44 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D86" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D86" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B87" t="n">
-        <v>22</v>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D87" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A87" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E87" s="2" t="n"/>
+      <c r="F87" s="2" t="n"/>
+      <c r="G87" s="2" t="n"/>
+      <c r="H87" s="2" t="n"/>
+      <c r="I87" s="2" t="n"/>
+      <c r="J87" s="2" t="n"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2492,7 +2712,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2512,7 +2732,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2532,16 +2752,16 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D90" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D90" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2552,7 +2772,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2572,7 +2792,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2592,16 +2812,16 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D93" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D93" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2612,7 +2832,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2632,7 +2852,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2652,38 +2872,44 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D96" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D96" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v>16</v>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D97" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A97" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B97" s="2" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E97" s="2" t="n"/>
+      <c r="F97" s="2" t="n"/>
+      <c r="G97" s="2" t="n"/>
+      <c r="H97" s="2" t="n"/>
+      <c r="I97" s="2" t="n"/>
+      <c r="J97" s="2" t="n"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2692,7 +2918,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2706,30 +2932,24 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B99" s="2" t="inlineStr">
-        <is>
-          <t>PR</t>
-        </is>
-      </c>
-      <c r="C99" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D99" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E99" s="2" t="n"/>
-      <c r="F99" s="2" t="n"/>
-      <c r="G99" s="2" t="n"/>
-      <c r="H99" s="2" t="n"/>
-      <c r="I99" s="2" t="n"/>
-      <c r="J99" s="2" t="n"/>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>97</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D99" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2738,16 +2958,16 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D100" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D100" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2758,16 +2978,16 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D101" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D101" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2778,16 +2998,16 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D102" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D102" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2798,7 +3018,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -2818,7 +3038,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -2838,64 +3058,64 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D105" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D105" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="inlineStr">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>84</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D106" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="inlineStr">
         <is>
           <t>Category :</t>
         </is>
       </c>
-      <c r="B106" s="2" t="inlineStr">
-        <is>
-          <t>GI</t>
-        </is>
-      </c>
-      <c r="C106" s="2" t="inlineStr">
+      <c r="B107" s="2" t="inlineStr">
+        <is>
+          <t>AG</t>
+        </is>
+      </c>
+      <c r="C107" s="2" t="inlineStr">
         <is>
           <t>Overall score :</t>
         </is>
       </c>
-      <c r="D106" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2" t="n"/>
-      <c r="F106" s="2" t="n"/>
-      <c r="G106" s="2" t="n"/>
-      <c r="H106" s="2" t="n"/>
-      <c r="I106" s="2" t="n"/>
-      <c r="J106" s="2" t="n"/>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B107" t="n">
-        <v>25</v>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D107" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="D107" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E107" s="2" t="n"/>
+      <c r="F107" s="2" t="n"/>
+      <c r="G107" s="2" t="n"/>
+      <c r="H107" s="2" t="n"/>
+      <c r="I107" s="2" t="n"/>
+      <c r="J107" s="2" t="n"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2904,7 +3124,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -2924,7 +3144,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2944,7 +3164,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -2964,7 +3184,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -2984,16 +3204,16 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D112" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D112" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3004,7 +3224,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -3024,16 +3244,16 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D114" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D114" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3044,7 +3264,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -3064,44 +3284,38 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D116" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D116" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B117" s="2" t="inlineStr">
-        <is>
-          <t>AN</t>
-        </is>
-      </c>
-      <c r="C117" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D117" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E117" s="2" t="n"/>
-      <c r="F117" s="2" t="n"/>
-      <c r="G117" s="2" t="n"/>
-      <c r="H117" s="2" t="n"/>
-      <c r="I117" s="2" t="n"/>
-      <c r="J117" s="2" t="n"/>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>27</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D117" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3110,7 +3324,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -3130,16 +3344,16 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D119" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D119" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3150,7 +3364,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -3170,38 +3384,44 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D121" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D121" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B122" t="n">
-        <v>47</v>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D122" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A122" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B122" s="2" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="C122" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D122" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E122" s="2" t="n"/>
+      <c r="F122" s="2" t="n"/>
+      <c r="G122" s="2" t="n"/>
+      <c r="H122" s="2" t="n"/>
+      <c r="I122" s="2" t="n"/>
+      <c r="J122" s="2" t="n"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3210,7 +3430,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3230,7 +3450,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3250,16 +3470,16 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D125" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D125" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3270,7 +3490,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -3290,64 +3510,64 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D127" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D127" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="inlineStr">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>92</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D128" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="inlineStr">
         <is>
           <t>Category :</t>
         </is>
       </c>
-      <c r="B128" s="2" t="inlineStr">
-        <is>
-          <t>AH</t>
-        </is>
-      </c>
-      <c r="C128" s="2" t="inlineStr">
+      <c r="B129" s="2" t="inlineStr">
+        <is>
+          <t>GI</t>
+        </is>
+      </c>
+      <c r="C129" s="2" t="inlineStr">
         <is>
           <t>Overall score :</t>
         </is>
       </c>
-      <c r="D128" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E128" s="2" t="n"/>
-      <c r="F128" s="2" t="n"/>
-      <c r="G128" s="2" t="n"/>
-      <c r="H128" s="2" t="n"/>
-      <c r="I128" s="2" t="n"/>
-      <c r="J128" s="2" t="n"/>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B129" t="n">
-        <v>45</v>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D129" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="D129" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E129" s="2" t="n"/>
+      <c r="F129" s="2" t="n"/>
+      <c r="G129" s="2" t="n"/>
+      <c r="H129" s="2" t="n"/>
+      <c r="I129" s="2" t="n"/>
+      <c r="J129" s="2" t="n"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3356,7 +3576,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -3376,7 +3596,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -3396,7 +3616,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -3416,16 +3636,16 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D133" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D133" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3436,16 +3656,16 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D134" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D134" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3456,16 +3676,16 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D135" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D135" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3476,7 +3696,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -3496,16 +3716,16 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D137" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D137" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3523,9 +3743,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D138" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D138" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3536,7 +3756,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -3557,7 +3777,7 @@
       </c>
       <c r="B140" s="2" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>AN</t>
         </is>
       </c>
       <c r="C140" s="2" t="inlineStr">
@@ -3566,7 +3786,7 @@
         </is>
       </c>
       <c r="D140" s="2" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E140" s="2" t="n"/>
       <c r="F140" s="2" t="n"/>
@@ -3582,16 +3802,16 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D141" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D141" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3602,7 +3822,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -3622,7 +3842,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
@@ -3642,16 +3862,16 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D144" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D144" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3662,16 +3882,16 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D145" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D145" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3682,7 +3902,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
@@ -3702,7 +3922,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
@@ -3722,7 +3942,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
@@ -3742,16 +3962,16 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D149" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D149" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3762,7 +3982,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
@@ -3776,24 +3996,30 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B151" t="n">
-        <v>91</v>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D151" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A151" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B151" s="2" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="C151" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D151" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E151" s="2" t="n"/>
+      <c r="F151" s="2" t="n"/>
+      <c r="G151" s="2" t="n"/>
+      <c r="H151" s="2" t="n"/>
+      <c r="I151" s="2" t="n"/>
+      <c r="J151" s="2" t="n"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3802,7 +4028,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
@@ -3822,7 +4048,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -3842,7 +4068,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
@@ -3862,7 +4088,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
@@ -3876,30 +4102,24 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B156" s="2" t="inlineStr">
-        <is>
-          <t>OD</t>
-        </is>
-      </c>
-      <c r="C156" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D156" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E156" s="2" t="n"/>
-      <c r="F156" s="2" t="n"/>
-      <c r="G156" s="2" t="n"/>
-      <c r="H156" s="2" t="n"/>
-      <c r="I156" s="2" t="n"/>
-      <c r="J156" s="2" t="n"/>
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>54</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D156" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3908,16 +4128,16 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D157" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D157" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3928,7 +4148,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
@@ -3948,16 +4168,16 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D159" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D159" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3968,16 +4188,16 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D160" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D160" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3988,16 +4208,16 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D161" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D161" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4008,38 +4228,44 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D162" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D162" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B163" t="n">
-        <v>59</v>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D163" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A163" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B163" s="2" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="C163" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D163" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E163" s="2" t="n"/>
+      <c r="F163" s="2" t="n"/>
+      <c r="G163" s="2" t="n"/>
+      <c r="H163" s="2" t="n"/>
+      <c r="I163" s="2" t="n"/>
+      <c r="J163" s="2" t="n"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4048,7 +4274,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
@@ -4062,30 +4288,24 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B165" s="2" t="inlineStr">
-        <is>
-          <t>PI</t>
-        </is>
-      </c>
-      <c r="C165" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D165" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E165" s="2" t="n"/>
-      <c r="F165" s="2" t="n"/>
-      <c r="G165" s="2" t="n"/>
-      <c r="H165" s="2" t="n"/>
-      <c r="I165" s="2" t="n"/>
-      <c r="J165" s="2" t="n"/>
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>65</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D165" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4094,7 +4314,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
@@ -4114,7 +4334,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
@@ -4134,7 +4354,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
@@ -4154,7 +4374,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
@@ -4174,16 +4394,16 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D170" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D170" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4194,7 +4414,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
@@ -4208,30 +4428,24 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B172" s="2" t="inlineStr">
-        <is>
-          <t>NI</t>
-        </is>
-      </c>
-      <c r="C172" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D172" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E172" s="2" t="n"/>
-      <c r="F172" s="2" t="n"/>
-      <c r="G172" s="2" t="n"/>
-      <c r="H172" s="2" t="n"/>
-      <c r="I172" s="2" t="n"/>
-      <c r="J172" s="2" t="n"/>
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>27</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D172" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -4240,7 +4454,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
@@ -4260,16 +4474,16 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D174" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D174" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4280,7 +4494,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
@@ -4300,16 +4514,16 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D176" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D176" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4320,7 +4534,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -4340,14 +4554,492 @@
         </is>
       </c>
       <c r="B178" t="n">
+        <v>96</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D178" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B179" s="2" t="inlineStr">
+        <is>
+          <t>OD</t>
+        </is>
+      </c>
+      <c r="C179" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D179" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E179" s="2" t="n"/>
+      <c r="F179" s="2" t="n"/>
+      <c r="G179" s="2" t="n"/>
+      <c r="H179" s="2" t="n"/>
+      <c r="I179" s="2" t="n"/>
+      <c r="J179" s="2" t="n"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>21</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D180" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>57</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D181" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>73</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D182" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>14</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D183" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>94</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D184" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>102</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D185" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>59</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D186" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>48</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D187" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B188" s="2" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="C188" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D188" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E188" s="2" t="n"/>
+      <c r="F188" s="2" t="n"/>
+      <c r="G188" s="2" t="n"/>
+      <c r="H188" s="2" t="n"/>
+      <c r="I188" s="2" t="n"/>
+      <c r="J188" s="2" t="n"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>33</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D189" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>105</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D190" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>38</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D191" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>74</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D192" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>31</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D193" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>80</v>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D194" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B195" s="2" t="inlineStr">
+        <is>
+          <t>NI</t>
+        </is>
+      </c>
+      <c r="C195" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D195" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E195" s="2" t="n"/>
+      <c r="F195" s="2" t="n"/>
+      <c r="G195" s="2" t="n"/>
+      <c r="H195" s="2" t="n"/>
+      <c r="I195" s="2" t="n"/>
+      <c r="J195" s="2" t="n"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>1</v>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D196" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>18</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D197" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>26</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D198" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>42</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D199" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>8</v>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D200" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
         <v>32</v>
       </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D178" s="3" t="inlineStr">
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D201" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Refactor Survey class to add conditional cell fill based on question number in app.py
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -59,14 +59,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fccf45"/>
-        <bgColor rgb="00fccf45"/>
+        <fgColor rgb="00fd1de9"/>
+        <bgColor rgb="00fd1de9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fd1de9"/>
-        <bgColor rgb="00fd1de9"/>
+        <fgColor rgb="00fccf45"/>
+        <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
   </fills>
@@ -501,7 +501,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Thu Apr 18 12:52:19 2024</t>
+          <t>Thu Apr 18 19:45:37 2024</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>99 %</t>
+          <t>11 %</t>
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
@@ -565,9 +565,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -605,9 +605,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -625,9 +625,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -645,9 +645,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -665,9 +665,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D9" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -705,9 +705,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D11" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -725,9 +725,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D12" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
       <c r="J13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="4" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
@@ -769,9 +769,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D14" s="6" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D15" s="6" t="inlineStr">
+      <c r="D15" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -816,7 +816,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="6" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
@@ -829,7 +829,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D16" s="6" t="inlineStr">
+      <c r="D16" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -859,7 +859,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D17" s="6" t="inlineStr">
+      <c r="D17" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -876,7 +876,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="4" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
@@ -889,7 +889,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D18" s="6" t="inlineStr">
+      <c r="D18" s="3" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -901,7 +901,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -919,9 +919,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D20" s="6" t="inlineStr">
+      <c r="D20" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -979,9 +979,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D21" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1009,9 +1009,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1021,12 +1021,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="6" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
@@ -1039,9 +1039,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D23" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1069,9 +1069,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D24" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
@@ -1123,9 +1123,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D26" s="3" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D27" s="6" t="inlineStr">
+      <c r="D27" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1183,7 +1183,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D28" s="6" t="inlineStr">
+      <c r="D28" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1213,9 +1213,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D29" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1243,9 +1243,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D30" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1255,12 +1255,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="6" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
@@ -1273,7 +1273,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D31" s="6" t="inlineStr">
+      <c r="D31" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1303,7 +1303,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D32" s="6" t="inlineStr">
+      <c r="D32" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1333,7 +1333,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D33" s="6" t="inlineStr">
+      <c r="D33" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1350,7 +1350,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="6" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
@@ -1363,9 +1363,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D34" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D34" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1393,7 +1393,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D35" s="6" t="inlineStr">
+      <c r="D35" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1416,7 +1416,7 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D37" s="6" t="inlineStr">
+      <c r="D37" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1477,7 +1477,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D38" s="6" t="inlineStr">
+      <c r="D38" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1507,7 +1507,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D39" s="6" t="inlineStr">
+      <c r="D39" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1537,7 +1537,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D40" s="6" t="inlineStr">
+      <c r="D40" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1567,7 +1567,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D41" s="6" t="inlineStr">
+      <c r="D41" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1597,9 +1597,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D42" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D42" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1627,9 +1627,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D43" s="3" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D43" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1657,9 +1657,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D44" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D44" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
@@ -1711,7 +1711,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D46" s="6" t="inlineStr">
+      <c r="D46" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1741,7 +1741,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D47" s="6" t="inlineStr">
+      <c r="D47" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1771,7 +1771,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D48" s="6" t="inlineStr">
+      <c r="D48" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1801,7 +1801,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D49" s="6" t="inlineStr">
+      <c r="D49" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1831,7 +1831,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D50" s="6" t="inlineStr">
+      <c r="D50" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1861,7 +1861,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D51" s="6" t="inlineStr">
+      <c r="D51" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1891,9 +1891,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D52" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D52" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -1921,7 +1921,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D53" s="6" t="inlineStr">
+      <c r="D53" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1951,7 +1951,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D54" s="6" t="inlineStr">
+      <c r="D54" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1981,7 +1981,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D55" s="6" t="inlineStr">
+      <c r="D55" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2011,9 +2011,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D56" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D56" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2041,7 +2041,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D57" s="6" t="inlineStr">
+      <c r="D57" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2071,9 +2071,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D58" s="3" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D58" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D59" s="6" t="inlineStr">
+      <c r="D59" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2131,7 +2131,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D60" s="6" t="inlineStr">
+      <c r="D60" s="5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2164,7 +2164,7 @@
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E61" s="2" t="n"/>
       <c r="F61" s="2" t="n"/>
@@ -2207,9 +2207,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D63" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D63" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2247,9 +2247,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D65" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D65" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2267,9 +2267,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D66" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D66" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2367,9 +2367,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D71" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D71" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2390,7 @@
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E72" s="2" t="n"/>
       <c r="F72" s="2" t="n"/>
@@ -2413,9 +2413,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D73" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2493,9 +2493,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D77" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D77" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D78" s="5" t="inlineStr">
+      <c r="D78" s="6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2533,9 +2533,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D79" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D79" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2573,9 +2573,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D81" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D81" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2593,9 +2593,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D82" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D82" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2613,9 +2613,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D83" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D83" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2633,9 +2633,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D84" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D84" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2653,9 +2653,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D85" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D85" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2673,9 +2673,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D86" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D86" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2696,7 +2696,7 @@
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E87" s="2" t="n"/>
       <c r="F87" s="2" t="n"/>
@@ -2759,9 +2759,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D90" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D90" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2819,9 +2819,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D93" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D93" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2879,9 +2879,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D96" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D96" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E97" s="2" t="n"/>
       <c r="F97" s="2" t="n"/>
@@ -2945,9 +2945,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D99" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D99" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2965,9 +2965,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D100" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D100" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2985,9 +2985,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D101" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3005,9 +3005,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D102" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D102" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3065,9 +3065,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D105" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D105" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3108,7 +3108,7 @@
         </is>
       </c>
       <c r="D107" s="2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E107" s="2" t="n"/>
       <c r="F107" s="2" t="n"/>
@@ -3211,9 +3211,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D112" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D112" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3251,9 +3251,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D114" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D114" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3291,9 +3291,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D116" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D116" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3351,9 +3351,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D119" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D119" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3391,9 +3391,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D121" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D121" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3414,7 +3414,7 @@
         </is>
       </c>
       <c r="D122" s="2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E122" s="2" t="n"/>
       <c r="F122" s="2" t="n"/>
@@ -3477,9 +3477,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D125" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D125" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3517,9 +3517,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D127" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D127" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3537,9 +3537,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D128" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D128" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3560,7 +3560,7 @@
         </is>
       </c>
       <c r="D129" s="2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E129" s="2" t="n"/>
       <c r="F129" s="2" t="n"/>
@@ -3643,9 +3643,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D133" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D133" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3663,9 +3663,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D134" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D134" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3683,9 +3683,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D135" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D135" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3723,9 +3723,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D137" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D137" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3743,9 +3743,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D138" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D138" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
         </is>
       </c>
       <c r="D140" s="2" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E140" s="2" t="n"/>
       <c r="F140" s="2" t="n"/>
@@ -3809,9 +3809,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D141" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D141" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3869,9 +3869,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D144" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D144" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3889,9 +3889,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D145" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D145" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3969,9 +3969,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D149" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D149" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4012,7 +4012,7 @@
         </is>
       </c>
       <c r="D151" s="2" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E151" s="2" t="n"/>
       <c r="F151" s="2" t="n"/>
@@ -4035,9 +4035,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D152" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D152" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4115,7 +4115,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D156" s="5" t="inlineStr">
+      <c r="D156" s="6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -4135,9 +4135,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D157" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D157" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4175,9 +4175,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D159" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D159" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4195,9 +4195,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D160" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D160" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4215,9 +4215,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D161" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D161" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4235,9 +4235,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D162" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D162" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4258,7 +4258,7 @@
         </is>
       </c>
       <c r="D163" s="2" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E163" s="2" t="n"/>
       <c r="F163" s="2" t="n"/>
@@ -4401,9 +4401,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D170" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D170" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4481,9 +4481,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D174" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D174" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4521,9 +4521,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D176" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D176" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4584,7 +4584,7 @@
         </is>
       </c>
       <c r="D179" s="2" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E179" s="2" t="n"/>
       <c r="F179" s="2" t="n"/>
@@ -4707,9 +4707,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D185" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D185" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4727,9 +4727,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D186" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D186" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4747,9 +4747,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D187" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D187" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4770,7 +4770,7 @@
         </is>
       </c>
       <c r="D188" s="2" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E188" s="2" t="n"/>
       <c r="F188" s="2" t="n"/>
@@ -4793,9 +4793,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D189" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D189" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4813,9 +4813,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D190" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="D190" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4853,9 +4853,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D192" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D192" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4893,9 +4893,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D194" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="D194" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4916,7 +4916,7 @@
         </is>
       </c>
       <c r="D195" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E195" s="2" t="n"/>
       <c r="F195" s="2" t="n"/>
@@ -4999,9 +4999,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D199" s="5" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D199" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor Survey class to add self evaluation test for ADHD in app.py
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -53,6 +53,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00fccf45"/>
+        <bgColor rgb="00fccf45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00fd4343"/>
         <bgColor rgb="00fd4343"/>
       </patternFill>
@@ -61,12 +67,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00fd1de9"/>
         <bgColor rgb="00fd1de9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fccf45"/>
-        <bgColor rgb="00fccf45"/>
       </patternFill>
     </fill>
   </fills>
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J201"/>
+  <dimension ref="A1:L190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,42 +466,52 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Type of Test</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Self Evaluation</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name :</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr"/>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Age :</t>
         </is>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="F1" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Sex :</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Description :</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr"/>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr"/>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Time of creation :</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Thu Apr 18 19:45:37 2024</t>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Tue Apr 23 18:38:13 2024</t>
         </is>
       </c>
     </row>
@@ -512,7 +522,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -521,7 +531,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>11 %</t>
+          <t>97 %</t>
         </is>
       </c>
       <c r="E2" s="2" t="n"/>
@@ -530,6 +540,8 @@
       <c r="H2" s="2" t="n"/>
       <c r="I2" s="2" t="n"/>
       <c r="J2" s="2" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -538,7 +550,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -558,16 +570,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -578,16 +590,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -598,7 +610,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -618,16 +630,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -638,16 +650,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -658,16 +670,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -678,16 +690,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -698,16 +710,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -718,16 +730,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -738,15 +750,15 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>ADHD Hyperactivity :</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>ADHD Hyperactivity :</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
       </c>
       <c r="E13" s="2" t="n"/>
       <c r="F13" s="2" t="n"/>
@@ -754,24 +766,26 @@
       <c r="H13" s="2" t="n"/>
       <c r="I13" s="2" t="n"/>
       <c r="J13" s="2" t="n"/>
+      <c r="K13" s="2" t="n"/>
+      <c r="L13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -781,7 +795,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
     </row>
@@ -792,14 +806,14 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D15" s="5" t="inlineStr">
+      <c r="D15" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -816,22 +830,22 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D16" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -841,27 +855,27 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D17" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -871,7 +885,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -882,7 +896,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -891,7 +905,7 @@
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -912,16 +926,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D19" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -931,27 +945,27 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="5" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D20" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -961,27 +975,27 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="4" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D21" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -991,7 +1005,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1002,16 +1016,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D22" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1021,27 +1035,27 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D23" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1051,7 +1065,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1062,16 +1076,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D24" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1081,7 +1095,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1106,7 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
@@ -1100,7 +1114,7 @@
         </is>
       </c>
       <c r="D25" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="2" t="n"/>
       <c r="F25" s="2" t="n"/>
@@ -1108,6 +1122,8 @@
       <c r="H25" s="2" t="n"/>
       <c r="I25" s="2" t="n"/>
       <c r="J25" s="2" t="n"/>
+      <c r="K25" s="2" t="n"/>
+      <c r="L25" s="2" t="n"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1116,14 +1132,14 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D26" s="5" t="inlineStr">
+      <c r="D26" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1140,22 +1156,22 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D27" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1165,7 +1181,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1176,16 +1192,16 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D28" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1195,27 +1211,27 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D29" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1225,7 +1241,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1236,16 +1252,16 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D30" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1255,27 +1271,27 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D31" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D31" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1285,27 +1301,27 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="4" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D32" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1315,27 +1331,27 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="4" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D33" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1345,27 +1361,27 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Question number :</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D34" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D34" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1386,16 +1402,16 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D35" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D35" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1405,63 +1421,65 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="inlineStr">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>32</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>Oppositional defiant disorder score :</t>
         </is>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B37" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>Oppositional defiant disorder :</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C36" s="2" t="inlineStr">
-        <is>
-          <t>Oppositional defiant disorder :</t>
-        </is>
-      </c>
-      <c r="D36" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="2" t="n"/>
-      <c r="F36" s="2" t="n"/>
-      <c r="G36" s="2" t="n"/>
-      <c r="H36" s="2" t="n"/>
-      <c r="I36" s="2" t="n"/>
-      <c r="J36" s="2" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>21</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D37" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Evaluated :</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
+      <c r="E37" s="2" t="n"/>
+      <c r="F37" s="2" t="n"/>
+      <c r="G37" s="2" t="n"/>
+      <c r="H37" s="2" t="n"/>
+      <c r="I37" s="2" t="n"/>
+      <c r="J37" s="2" t="n"/>
+      <c r="K37" s="2" t="n"/>
+      <c r="L37" s="2" t="n"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1470,16 +1488,16 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D38" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D38" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1489,7 +1507,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1500,16 +1518,16 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D39" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D39" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1530,16 +1548,16 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D40" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D40" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1567,9 +1585,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D41" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D41" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1590,16 +1608,16 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>102</v>
+        <v>3</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D42" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D42" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1620,16 +1638,16 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D43" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1639,7 +1657,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1650,16 +1668,16 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D44" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D44" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1674,58 +1692,60 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="inlineStr">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>24</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Evaluated :</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
         <is>
           <t>Behavior disorder score :</t>
         </is>
       </c>
-      <c r="B45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C45" s="2" t="inlineStr">
+      <c r="B46" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
         <is>
           <t>Behavior disorder :</t>
         </is>
       </c>
-      <c r="D45" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="n"/>
-      <c r="F45" s="2" t="n"/>
-      <c r="G45" s="2" t="n"/>
-      <c r="H45" s="2" t="n"/>
-      <c r="I45" s="2" t="n"/>
-      <c r="J45" s="2" t="n"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>41</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D46" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Evaluated :</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
+      <c r="D46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="n"/>
+      <c r="F46" s="2" t="n"/>
+      <c r="G46" s="2" t="n"/>
+      <c r="H46" s="2" t="n"/>
+      <c r="I46" s="2" t="n"/>
+      <c r="J46" s="2" t="n"/>
+      <c r="K46" s="2" t="n"/>
+      <c r="L46" s="2" t="n"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1734,16 +1754,16 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D47" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1753,7 +1773,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1764,16 +1784,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D48" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1783,7 +1803,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1794,14 +1814,14 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D49" s="5" t="inlineStr">
+      <c r="D49" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1824,16 +1844,16 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D50" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1843,7 +1863,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1854,16 +1874,16 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D51" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1873,7 +1893,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1884,16 +1904,16 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D52" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1903,7 +1923,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1914,16 +1934,16 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D53" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1933,7 +1953,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1944,16 +1964,16 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D54" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1963,7 +1983,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1974,14 +1994,14 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D55" s="5" t="inlineStr">
+      <c r="D55" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2011,9 +2031,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D56" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D56" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2023,7 +2043,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -2034,14 +2054,14 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D57" s="5" t="inlineStr">
+      <c r="D57" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2064,16 +2084,16 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D58" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2083,7 +2103,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -2094,16 +2114,16 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D59" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2113,7 +2133,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -2124,16 +2144,16 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D60" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D60" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2143,7 +2163,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -2164,7 +2184,7 @@
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E61" s="2" t="n"/>
       <c r="F61" s="2" t="n"/>
@@ -2172,6 +2192,8 @@
       <c r="H61" s="2" t="n"/>
       <c r="I61" s="2" t="n"/>
       <c r="J61" s="2" t="n"/>
+      <c r="K61" s="2" t="n"/>
+      <c r="L61" s="2" t="n"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2207,9 +2229,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D63" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D63" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2227,9 +2249,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D64" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D64" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2247,9 +2269,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D65" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2267,9 +2289,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D66" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D66" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2287,9 +2309,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D67" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D67" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2307,9 +2329,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D68" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D68" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2327,9 +2349,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D69" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D69" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2347,9 +2369,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D70" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D70" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2367,9 +2389,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D71" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D71" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2412,7 @@
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E72" s="2" t="n"/>
       <c r="F72" s="2" t="n"/>
@@ -2398,6 +2420,8 @@
       <c r="H72" s="2" t="n"/>
       <c r="I72" s="2" t="n"/>
       <c r="J72" s="2" t="n"/>
+      <c r="K72" s="2" t="n"/>
+      <c r="L72" s="2" t="n"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2413,9 +2437,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D73" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D73" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2433,9 +2457,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D74" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D74" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2453,9 +2477,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D75" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D75" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2493,9 +2517,9 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D77" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D77" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2513,7 +2537,7 @@
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D78" s="6" t="inlineStr">
+      <c r="D78" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -2526,16 +2550,16 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D79" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D79" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2546,16 +2570,16 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D80" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D80" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2566,16 +2590,16 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D81" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D81" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2586,16 +2610,16 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D82" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D82" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2606,38 +2630,46 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D83" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D83" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
-        <v>99</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D84" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E84" s="2" t="n"/>
+      <c r="F84" s="2" t="n"/>
+      <c r="G84" s="2" t="n"/>
+      <c r="H84" s="2" t="n"/>
+      <c r="I84" s="2" t="n"/>
+      <c r="J84" s="2" t="n"/>
+      <c r="K84" s="2" t="n"/>
+      <c r="L84" s="2" t="n"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2646,7 +2678,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2666,7 +2698,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2680,30 +2712,24 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B87" s="2" t="inlineStr">
-        <is>
-          <t>LP</t>
-        </is>
-      </c>
-      <c r="C87" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D87" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E87" s="2" t="n"/>
-      <c r="F87" s="2" t="n"/>
-      <c r="G87" s="2" t="n"/>
-      <c r="H87" s="2" t="n"/>
-      <c r="I87" s="2" t="n"/>
-      <c r="J87" s="2" t="n"/>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>53</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D87" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2712,7 +2738,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2732,16 +2758,16 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D89" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D89" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2752,16 +2778,16 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D90" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D90" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2772,16 +2798,16 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D91" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D91" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2792,16 +2818,16 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D92" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D92" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2812,38 +2838,46 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D93" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D93" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>87</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D94" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>EF</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E94" s="2" t="n"/>
+      <c r="F94" s="2" t="n"/>
+      <c r="G94" s="2" t="n"/>
+      <c r="H94" s="2" t="n"/>
+      <c r="I94" s="2" t="n"/>
+      <c r="J94" s="2" t="n"/>
+      <c r="K94" s="2" t="n"/>
+      <c r="L94" s="2" t="n"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2852,7 +2886,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2872,44 +2906,38 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D96" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D96" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B97" s="2" t="inlineStr">
-        <is>
-          <t>EF</t>
-        </is>
-      </c>
-      <c r="C97" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D97" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="n"/>
-      <c r="F97" s="2" t="n"/>
-      <c r="G97" s="2" t="n"/>
-      <c r="H97" s="2" t="n"/>
-      <c r="I97" s="2" t="n"/>
-      <c r="J97" s="2" t="n"/>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>34</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D97" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2918,7 +2946,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2938,16 +2966,16 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D99" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D99" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2958,16 +2986,16 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D100" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D100" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2978,16 +3006,16 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D101" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D101" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2998,16 +3026,16 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D102" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D102" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3018,38 +3046,46 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D103" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D103" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B104" t="n">
-        <v>79</v>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D104" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>AG</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="E104" s="2" t="n"/>
+      <c r="F104" s="2" t="n"/>
+      <c r="G104" s="2" t="n"/>
+      <c r="H104" s="2" t="n"/>
+      <c r="I104" s="2" t="n"/>
+      <c r="J104" s="2" t="n"/>
+      <c r="K104" s="2" t="n"/>
+      <c r="L104" s="2" t="n"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3058,7 +3094,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -3078,44 +3114,38 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D106" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D106" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B107" s="2" t="inlineStr">
-        <is>
-          <t>AG</t>
-        </is>
-      </c>
-      <c r="C107" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D107" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="n"/>
-      <c r="F107" s="2" t="n"/>
-      <c r="G107" s="2" t="n"/>
-      <c r="H107" s="2" t="n"/>
-      <c r="I107" s="2" t="n"/>
-      <c r="J107" s="2" t="n"/>
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>22</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D107" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3124,16 +3154,16 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D108" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D108" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3144,16 +3174,16 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D109" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D109" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3164,16 +3194,16 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D110" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D110" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3184,16 +3214,16 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D111" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D111" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3204,16 +3234,16 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D112" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D112" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3224,16 +3254,16 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D113" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D113" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3244,16 +3274,16 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D114" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D114" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3264,16 +3294,16 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D115" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D115" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3284,16 +3314,16 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D116" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D116" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3304,38 +3334,46 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D117" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D117" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B118" t="n">
-        <v>39</v>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D118" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A118" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B118" s="2" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="C118" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D118" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E118" s="2" t="n"/>
+      <c r="F118" s="2" t="n"/>
+      <c r="G118" s="2" t="n"/>
+      <c r="H118" s="2" t="n"/>
+      <c r="I118" s="2" t="n"/>
+      <c r="J118" s="2" t="n"/>
+      <c r="K118" s="2" t="n"/>
+      <c r="L118" s="2" t="n"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3344,16 +3382,16 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D119" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D119" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3364,16 +3402,16 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D120" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D120" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3384,44 +3422,38 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D121" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D121" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B122" s="2" t="inlineStr">
-        <is>
-          <t>PR</t>
-        </is>
-      </c>
-      <c r="C122" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D122" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E122" s="2" t="n"/>
-      <c r="F122" s="2" t="n"/>
-      <c r="G122" s="2" t="n"/>
-      <c r="H122" s="2" t="n"/>
-      <c r="I122" s="2" t="n"/>
-      <c r="J122" s="2" t="n"/>
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>24</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D122" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3430,16 +3462,16 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D123" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D123" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3450,38 +3482,46 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D124" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D124" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B125" t="n">
-        <v>62</v>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D125" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A125" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B125" s="2" t="inlineStr">
+        <is>
+          <t>GI</t>
+        </is>
+      </c>
+      <c r="C125" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D125" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E125" s="2" t="n"/>
+      <c r="F125" s="2" t="n"/>
+      <c r="G125" s="2" t="n"/>
+      <c r="H125" s="2" t="n"/>
+      <c r="I125" s="2" t="n"/>
+      <c r="J125" s="2" t="n"/>
+      <c r="K125" s="2" t="n"/>
+      <c r="L125" s="2" t="n"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3490,16 +3530,16 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D126" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D126" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3510,16 +3550,16 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D127" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D127" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3530,44 +3570,38 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D128" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D128" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B129" s="2" t="inlineStr">
-        <is>
-          <t>GI</t>
-        </is>
-      </c>
-      <c r="C129" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D129" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E129" s="2" t="n"/>
-      <c r="F129" s="2" t="n"/>
-      <c r="G129" s="2" t="n"/>
-      <c r="H129" s="2" t="n"/>
-      <c r="I129" s="2" t="n"/>
-      <c r="J129" s="2" t="n"/>
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>85</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D129" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3576,16 +3610,16 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D130" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D130" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3596,16 +3630,16 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D131" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D131" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3616,16 +3650,16 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D132" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D132" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3636,16 +3670,16 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D133" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D133" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3656,38 +3690,46 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D134" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D134" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B135" t="n">
-        <v>50</v>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D135" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A135" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B135" s="2" t="inlineStr">
+        <is>
+          <t>AN</t>
+        </is>
+      </c>
+      <c r="C135" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D135" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E135" s="2" t="n"/>
+      <c r="F135" s="2" t="n"/>
+      <c r="G135" s="2" t="n"/>
+      <c r="H135" s="2" t="n"/>
+      <c r="I135" s="2" t="n"/>
+      <c r="J135" s="2" t="n"/>
+      <c r="K135" s="2" t="n"/>
+      <c r="L135" s="2" t="n"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3696,16 +3738,16 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D136" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D136" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3716,16 +3758,16 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D137" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D137" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3736,16 +3778,16 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D138" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D138" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3756,44 +3798,38 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D139" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D139" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B140" s="2" t="inlineStr">
-        <is>
-          <t>AN</t>
-        </is>
-      </c>
-      <c r="C140" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D140" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E140" s="2" t="n"/>
-      <c r="F140" s="2" t="n"/>
-      <c r="G140" s="2" t="n"/>
-      <c r="H140" s="2" t="n"/>
-      <c r="I140" s="2" t="n"/>
-      <c r="J140" s="2" t="n"/>
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>79</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D140" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3802,16 +3838,16 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D141" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D141" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3822,16 +3858,16 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D142" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D142" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3842,16 +3878,16 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D143" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D143" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -3862,38 +3898,46 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D144" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D144" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B145" t="n">
-        <v>47</v>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D145" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A145" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B145" s="2" t="inlineStr">
+        <is>
+          <t>AH</t>
+        </is>
+      </c>
+      <c r="C145" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D145" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E145" s="2" t="n"/>
+      <c r="F145" s="2" t="n"/>
+      <c r="G145" s="2" t="n"/>
+      <c r="H145" s="2" t="n"/>
+      <c r="I145" s="2" t="n"/>
+      <c r="J145" s="2" t="n"/>
+      <c r="K145" s="2" t="n"/>
+      <c r="L145" s="2" t="n"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3902,7 +3946,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
@@ -3922,16 +3966,16 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D147" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D147" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -3942,16 +3986,16 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D148" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D148" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -3962,7 +4006,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
@@ -3982,44 +4026,38 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D150" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D150" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B151" s="2" t="inlineStr">
-        <is>
-          <t>AH</t>
-        </is>
-      </c>
-      <c r="C151" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D151" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E151" s="2" t="n"/>
-      <c r="F151" s="2" t="n"/>
-      <c r="G151" s="2" t="n"/>
-      <c r="H151" s="2" t="n"/>
-      <c r="I151" s="2" t="n"/>
-      <c r="J151" s="2" t="n"/>
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>3</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D151" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -4028,16 +4066,16 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D152" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="D152" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4048,38 +4086,46 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D153" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D153" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B154" t="n">
-        <v>69</v>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D154" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A154" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B154" s="2" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="C154" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D154" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="E154" s="2" t="n"/>
+      <c r="F154" s="2" t="n"/>
+      <c r="G154" s="2" t="n"/>
+      <c r="H154" s="2" t="n"/>
+      <c r="I154" s="2" t="n"/>
+      <c r="J154" s="2" t="n"/>
+      <c r="K154" s="2" t="n"/>
+      <c r="L154" s="2" t="n"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -4088,7 +4134,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
@@ -4108,14 +4154,14 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C156" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D156" s="6" t="inlineStr">
+      <c r="D156" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -4128,16 +4174,16 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D157" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D157" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4148,7 +4194,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
@@ -4168,16 +4214,16 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D159" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D159" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4188,16 +4234,16 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D160" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D160" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4208,16 +4254,16 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D161" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D161" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4228,44 +4274,38 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D162" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D162" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B163" s="2" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="C163" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D163" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E163" s="2" t="n"/>
-      <c r="F163" s="2" t="n"/>
-      <c r="G163" s="2" t="n"/>
-      <c r="H163" s="2" t="n"/>
-      <c r="I163" s="2" t="n"/>
-      <c r="J163" s="2" t="n"/>
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>27</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D163" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4274,16 +4314,16 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D164" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D164" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4294,16 +4334,16 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D165" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D165" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4314,16 +4354,16 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D166" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D166" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4334,16 +4374,16 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D167" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D167" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4354,16 +4394,16 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D168" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D168" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -4374,7 +4414,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
@@ -4388,24 +4428,32 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B170" t="n">
-        <v>78</v>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D170" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A170" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B170" s="2" t="inlineStr">
+        <is>
+          <t>OD</t>
+        </is>
+      </c>
+      <c r="C170" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D170" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E170" s="2" t="n"/>
+      <c r="F170" s="2" t="n"/>
+      <c r="G170" s="2" t="n"/>
+      <c r="H170" s="2" t="n"/>
+      <c r="I170" s="2" t="n"/>
+      <c r="J170" s="2" t="n"/>
+      <c r="K170" s="2" t="n"/>
+      <c r="L170" s="2" t="n"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -4414,16 +4462,16 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D171" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D171" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4434,7 +4482,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -4454,16 +4502,16 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D173" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D173" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4474,16 +4522,16 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D174" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D174" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4494,16 +4542,16 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D175" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D175" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4514,7 +4562,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -4534,64 +4582,66 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D177" s="3" t="inlineStr">
+      <c r="D177" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B178" s="2" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="C178" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D178" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E178" s="2" t="n"/>
+      <c r="F178" s="2" t="n"/>
+      <c r="G178" s="2" t="n"/>
+      <c r="H178" s="2" t="n"/>
+      <c r="I178" s="2" t="n"/>
+      <c r="J178" s="2" t="n"/>
+      <c r="K178" s="2" t="n"/>
+      <c r="L178" s="2" t="n"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>33</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D179" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B178" t="n">
-        <v>96</v>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D178" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B179" s="2" t="inlineStr">
-        <is>
-          <t>OD</t>
-        </is>
-      </c>
-      <c r="C179" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D179" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E179" s="2" t="n"/>
-      <c r="F179" s="2" t="n"/>
-      <c r="G179" s="2" t="n"/>
-      <c r="H179" s="2" t="n"/>
-      <c r="I179" s="2" t="n"/>
-      <c r="J179" s="2" t="n"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4600,16 +4650,16 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D180" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D180" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4620,16 +4670,16 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D181" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D181" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4640,16 +4690,16 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D182" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D182" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -4660,38 +4710,46 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D183" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D183" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B184" t="n">
-        <v>94</v>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D184" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A184" s="2" t="inlineStr">
+        <is>
+          <t>Category :</t>
+        </is>
+      </c>
+      <c r="B184" s="2" t="inlineStr">
+        <is>
+          <t>NI</t>
+        </is>
+      </c>
+      <c r="C184" s="2" t="inlineStr">
+        <is>
+          <t>Overall score :</t>
+        </is>
+      </c>
+      <c r="D184" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E184" s="2" t="n"/>
+      <c r="F184" s="2" t="n"/>
+      <c r="G184" s="2" t="n"/>
+      <c r="H184" s="2" t="n"/>
+      <c r="I184" s="2" t="n"/>
+      <c r="J184" s="2" t="n"/>
+      <c r="K184" s="2" t="n"/>
+      <c r="L184" s="2" t="n"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -4700,16 +4758,16 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="C185" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D185" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D185" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4720,16 +4778,16 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D186" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D186" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -4740,44 +4798,38 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C187" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D187" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D187" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B188" s="2" t="inlineStr">
-        <is>
-          <t>PI</t>
-        </is>
-      </c>
-      <c r="C188" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D188" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E188" s="2" t="n"/>
-      <c r="F188" s="2" t="n"/>
-      <c r="G188" s="2" t="n"/>
-      <c r="H188" s="2" t="n"/>
-      <c r="I188" s="2" t="n"/>
-      <c r="J188" s="2" t="n"/>
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Question number :</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>42</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Answer value :</t>
+        </is>
+      </c>
+      <c r="D188" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4786,7 +4838,7 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
@@ -4806,242 +4858,16 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="C190" t="inlineStr">
         <is>
           <t>Answer value :</t>
         </is>
       </c>
-      <c r="D190" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B191" t="n">
-        <v>38</v>
-      </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D191" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B192" t="n">
-        <v>74</v>
-      </c>
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D192" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B193" t="n">
-        <v>31</v>
-      </c>
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D193" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B194" t="n">
-        <v>80</v>
-      </c>
-      <c r="C194" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D194" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="2" t="inlineStr">
-        <is>
-          <t>Category :</t>
-        </is>
-      </c>
-      <c r="B195" s="2" t="inlineStr">
-        <is>
-          <t>NI</t>
-        </is>
-      </c>
-      <c r="C195" s="2" t="inlineStr">
-        <is>
-          <t>Overall score :</t>
-        </is>
-      </c>
-      <c r="D195" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E195" s="2" t="n"/>
-      <c r="F195" s="2" t="n"/>
-      <c r="G195" s="2" t="n"/>
-      <c r="H195" s="2" t="n"/>
-      <c r="I195" s="2" t="n"/>
-      <c r="J195" s="2" t="n"/>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B196" t="n">
-        <v>1</v>
-      </c>
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D196" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B197" t="n">
-        <v>18</v>
-      </c>
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D197" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B198" t="n">
-        <v>26</v>
-      </c>
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D198" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B199" t="n">
-        <v>42</v>
-      </c>
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D199" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B200" t="n">
-        <v>8</v>
-      </c>
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D200" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>Question number :</t>
-        </is>
-      </c>
-      <c r="B201" t="n">
-        <v>32</v>
-      </c>
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>Answer value :</t>
-        </is>
-      </c>
-      <c r="D201" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="D190" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>